<commit_message>
updated results for q5
</commit_message>
<xml_diff>
--- a/pubmed_results_Q5_.xlsx
+++ b/pubmed_results_Q5_.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t xml:space="preserve">UA = uncompressed array, BD = bit aligned dictionary, OPT = optimal, Huffman</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Avg of 5 (sec)</t>
   </si>
   <si>
+    <t xml:space="preserve">Previous Avg</t>
+  </si>
+  <si>
     <t xml:space="preserve">UA – 0 threads</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">Huffman – 4 threads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">‘</t>
   </si>
   <si>
     <t xml:space="preserve">Author ID Q5</t>
@@ -117,7 +123,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,14 +144,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -379,20 +382,20 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+      <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.9387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1377551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="48.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.8673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="50.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="12.8673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -460,101 +463,116 @@
       <c r="G6" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="H6" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>7.81284</v>
+        <v>7.55618</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0.591823</v>
+        <v>0.575643</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>12.1274</v>
+        <v>11.7396</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>8.98868</v>
+        <v>8.69336</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>22.5655</v>
+        <v>21.7836</v>
       </c>
       <c r="G7" s="7" t="n">
         <f aca="false">SUM(B7:F7)/5</f>
-        <v>10.4172486</v>
+        <v>10.0696766</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>7.315</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6" t="n">
-        <v>10.7887</v>
+        <v>10.8046</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>0.7938</v>
+        <v>0.797618</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>16.7313</v>
+        <v>16.8076</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>12.3996</v>
+        <v>12.4762</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>31.3702</v>
+        <v>31.3996</v>
       </c>
       <c r="G8" s="7" t="n">
         <f aca="false">SUM(B8:F8)/5</f>
-        <v>14.41672</v>
+        <v>14.4571236</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>10.01</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="6" t="n">
-        <v>6.47208</v>
+        <v>6.22213</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>0.731499</v>
+        <v>0.685278</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>10.8908</v>
+        <v>10.7322</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>7.07394</v>
+        <v>6.82371</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v>19.1616</v>
+        <v>18.5434</v>
       </c>
       <c r="G9" s="7" t="n">
         <f aca="false">SUM(B9:F9)/5</f>
-        <v>8.8659838</v>
+        <v>8.6013436</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>6.086</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="6" t="n">
-        <v>4.6871</v>
+        <v>4.639</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>0.785314</v>
+        <v>0.764011</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>7.94567</v>
+        <v>7.69529</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>4.44253</v>
+        <v>4.40684</v>
       </c>
       <c r="F10" s="6" t="n">
-        <v>11.6432</v>
+        <v>11.3197</v>
       </c>
       <c r="G10" s="7" t="n">
         <f aca="false">SUM(B10:F10)/5</f>
-        <v>5.9007628</v>
+        <v>5.7649682</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>4.45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,101 +583,114 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="6" t="n">
-        <v>8.69355</v>
+        <v>8.22453</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>0.655369</v>
+        <v>0.623172</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>13.4973</v>
+        <v>12.8024</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>10.0115</v>
+        <v>9.46525</v>
       </c>
       <c r="F12" s="6" t="n">
-        <v>25.1221</v>
+        <v>23.8016</v>
       </c>
       <c r="G12" s="7" t="n">
         <f aca="false">SUM(B12:F12)/5</f>
-        <v>11.5959638</v>
+        <v>10.9833904</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>10.569</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="6" t="n">
-        <v>11.855</v>
+        <v>11.5725</v>
       </c>
       <c r="C13" s="6" t="n">
-        <v>0.870006</v>
+        <v>0.851371</v>
       </c>
       <c r="D13" s="6" t="n">
-        <v>18.341</v>
+        <v>17.9272</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>13.6092</v>
+        <v>13.2952</v>
       </c>
       <c r="F13" s="6" t="n">
-        <v>34.3898</v>
+        <v>33.5791</v>
       </c>
       <c r="G13" s="7" t="n">
         <f aca="false">SUM(B13:F13)/5</f>
-        <v>15.8130012</v>
+        <v>15.4450742</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>12.856</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="6" t="n">
-        <v>6.73396</v>
+        <v>6.56816</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>0.743737</v>
+        <v>0.72547</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>11.5551</v>
+        <v>11.2772</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>7.40508</v>
+        <v>7.19448</v>
       </c>
       <c r="F14" s="6" t="n">
-        <v>20.2099</v>
+        <v>19.6801</v>
       </c>
       <c r="G14" s="7" t="n">
         <f aca="false">SUM(B14:F14)/5</f>
-        <v>9.3295554</v>
+        <v>9.089082</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>7.917</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="6" t="n">
-        <v>4.89419</v>
+        <v>4.79187</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>0.835443</v>
+        <v>0.81537</v>
       </c>
       <c r="D15" s="6" t="n">
-        <v>8.16631</v>
+        <v>8.01944</v>
       </c>
       <c r="E15" s="6" t="n">
-        <v>4.58351</v>
+        <v>4.47075</v>
       </c>
       <c r="F15" s="6" t="n">
-        <v>12.1091</v>
+        <v>11.8721</v>
       </c>
       <c r="G15" s="7" t="n">
         <f aca="false">SUM(B15:F15)/5</f>
-        <v>6.1177106</v>
+        <v>5.993906</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>5.375</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,101 +701,114 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="6" t="n">
-        <v>8.68993</v>
+        <v>8.25264</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>0.649665</v>
+        <v>0.62192</v>
       </c>
       <c r="D17" s="6" t="n">
-        <v>13.4725</v>
+        <v>12.7877</v>
       </c>
       <c r="E17" s="6" t="n">
-        <v>9.99545</v>
+        <v>9.48984</v>
       </c>
       <c r="F17" s="6" t="n">
-        <v>25.0839</v>
+        <v>23.8029</v>
       </c>
       <c r="G17" s="7" t="n">
         <f aca="false">SUM(B17:F17)/5</f>
-        <v>11.578289</v>
+        <v>10.991</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>10.435</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="6" t="n">
-        <v>11.8702</v>
+        <v>11.5745</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>0.868265</v>
+        <v>0.848295</v>
       </c>
       <c r="D18" s="6" t="n">
-        <v>18.3349</v>
+        <v>17.9409</v>
       </c>
       <c r="E18" s="6" t="n">
-        <v>13.6275</v>
+        <v>13.3067</v>
       </c>
       <c r="F18" s="6" t="n">
-        <v>34.5035</v>
+        <v>33.6437</v>
       </c>
       <c r="G18" s="7" t="n">
         <f aca="false">SUM(B18:F18)/5</f>
-        <v>15.840873</v>
+        <v>15.462819</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>12.4</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="6" t="n">
-        <v>6.7432</v>
+        <v>6.58737</v>
       </c>
       <c r="C19" s="6" t="n">
-        <v>0.743114</v>
+        <v>0.727063</v>
       </c>
       <c r="D19" s="6" t="n">
-        <v>11.549</v>
+        <v>11.299</v>
       </c>
       <c r="E19" s="6" t="n">
-        <v>7.41444</v>
+        <v>7.24222</v>
       </c>
       <c r="F19" s="6" t="n">
-        <v>20.1876</v>
+        <v>19.7823</v>
       </c>
       <c r="G19" s="7" t="n">
         <f aca="false">SUM(B19:F19)/5</f>
-        <v>9.3274708</v>
+        <v>9.1275906</v>
+      </c>
+      <c r="H19" s="4" t="n">
+        <v>7.51</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" s="6" t="n">
-        <v>4.92997</v>
+        <v>4.90556</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>0.833906</v>
+        <v>0.828068</v>
       </c>
       <c r="D20" s="6" t="n">
-        <v>8.19628</v>
+        <v>8.19764</v>
       </c>
       <c r="E20" s="6" t="n">
-        <v>4.60619</v>
+        <v>4.6278</v>
       </c>
       <c r="F20" s="6" t="n">
-        <v>12.0723</v>
+        <v>12.0795</v>
       </c>
       <c r="G20" s="7" t="n">
         <f aca="false">SUM(B20:F20)/5</f>
-        <v>6.1277292</v>
+        <v>6.1277136</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <v>5.207</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,75 +819,131 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="7"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>68.1854</v>
+      </c>
+      <c r="C22" s="6" t="n">
+        <v>4.71387</v>
+      </c>
+      <c r="D22" s="6" t="n">
+        <v>105.489</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>78.3184</v>
+      </c>
+      <c r="F22" s="6" t="n">
+        <v>197.115</v>
+      </c>
       <c r="G22" s="7" t="n">
         <f aca="false">SUM(B22:F22)/5</f>
-        <v>0</v>
+        <v>90.764334</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <v>98.87</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>71.2541</v>
+      </c>
+      <c r="C23" s="6" t="n">
+        <v>4.95935</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>109.995</v>
+      </c>
+      <c r="E23" s="6" t="n">
+        <v>82.2915</v>
+      </c>
+      <c r="F23" s="6" t="n">
+        <v>207.405</v>
+      </c>
       <c r="G23" s="7" t="n">
         <f aca="false">SUM(B23:F23)/5</f>
-        <v>0</v>
+        <v>95.18099</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>102.888</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>40.1517</v>
+      </c>
+      <c r="C24" s="6" t="n">
+        <v>4.34393</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>68.6148</v>
+      </c>
+      <c r="E24" s="6" t="n">
+        <v>43.2355</v>
+      </c>
+      <c r="F24" s="6" t="n">
+        <v>117.592</v>
+      </c>
       <c r="G24" s="7" t="n">
         <f aca="false">SUM(B24:F24)/5</f>
-        <v>0</v>
+        <v>54.787586</v>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>59.447</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>29.0818</v>
+      </c>
+      <c r="C25" s="6" t="n">
+        <v>4.86376</v>
+      </c>
+      <c r="D25" s="6" t="n">
+        <v>48.7242</v>
+      </c>
+      <c r="E25" s="6" t="n">
+        <v>27.0608</v>
+      </c>
+      <c r="F25" s="6" t="n">
+        <v>70.9214</v>
+      </c>
       <c r="G25" s="7" t="n">
         <f aca="false">SUM(B25:F25)/5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36.130392</v>
+      </c>
+      <c r="H25" s="4" t="n">
+        <v>39.421</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="8"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27" s="10" t="n">
         <v>10246893</v>
@@ -861,6 +961,7 @@
         <v>5450530</v>
       </c>
       <c r="G27" s="12"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
@@ -871,7 +972,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -897,10 +998,13 @@
       <c r="G31" s="14" t="s">
         <v>8</v>
       </c>
+      <c r="H31" s="14" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B32" s="15" t="n">
         <v>62.5008</v>
@@ -921,10 +1025,13 @@
         <f aca="false">SUM(B32:F32)/5</f>
         <v>94.01374</v>
       </c>
+      <c r="H32" s="13" t="n">
+        <v>59.476</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B33" s="15" t="n">
         <v>91.9048</v>
@@ -945,10 +1052,13 @@
         <f aca="false">SUM(B33:F33)/5</f>
         <v>138.2926</v>
       </c>
+      <c r="H33" s="13" t="n">
+        <v>87.212</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B34" s="15" t="n">
         <v>54.9212</v>
@@ -969,10 +1079,13 @@
         <f aca="false">SUM(B34:F34)/5</f>
         <v>81.12084</v>
       </c>
+      <c r="H34" s="13" t="n">
+        <v>55.25</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B35" s="15" t="n">
         <v>37.5282</v>
@@ -992,6 +1105,9 @@
       <c r="G35" s="16" t="n">
         <f aca="false">SUM(B35:F35)/5</f>
         <v>55.75058</v>
+      </c>
+      <c r="H35" s="13" t="n">
+        <v>42.084</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1002,10 +1118,11 @@
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
       <c r="G36" s="16"/>
+      <c r="H36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B37" s="15" t="n">
         <v>71.0241</v>
@@ -1026,10 +1143,13 @@
         <f aca="false">SUM(B37:F37)/5</f>
         <v>106.64854</v>
       </c>
+      <c r="H37" s="13" t="n">
+        <v>97.907</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B38" s="15" t="n">
         <v>99.458</v>
@@ -1050,10 +1170,13 @@
         <f aca="false">SUM(B38:F38)/5</f>
         <v>149.668</v>
       </c>
+      <c r="H38" s="13" t="n">
+        <v>117.104</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B39" s="15" t="n">
         <v>59.2424</v>
@@ -1074,10 +1197,13 @@
         <f aca="false">SUM(B39:F39)/5</f>
         <v>88.27344</v>
       </c>
+      <c r="H39" s="13" t="n">
+        <v>72.765</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B40" s="15" t="n">
         <v>39.8538</v>
@@ -1097,6 +1223,9 @@
       <c r="G40" s="16" t="n">
         <f aca="false">SUM(B40:F40)/5</f>
         <v>59.2086</v>
+      </c>
+      <c r="H40" s="13" t="n">
+        <v>51.133</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1107,10 +1236,11 @@
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
       <c r="G41" s="16"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B42" s="15" t="n">
         <v>69.5109</v>
@@ -1131,10 +1261,13 @@
         <f aca="false">SUM(B42:F42)/5</f>
         <v>104.32362</v>
       </c>
+      <c r="H42" s="13" t="n">
+        <v>91.984</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B43" s="15" t="n">
         <v>95.5823</v>
@@ -1155,10 +1288,13 @@
         <f aca="false">SUM(B43:F43)/5</f>
         <v>142.00664</v>
       </c>
+      <c r="H43" s="13" t="n">
+        <v>113.547</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B44" s="15" t="n">
         <v>55.951</v>
@@ -1179,10 +1315,13 @@
         <f aca="false">SUM(B44:F44)/5</f>
         <v>85.41982</v>
       </c>
+      <c r="H44" s="13" t="n">
+        <v>71.137</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B45" s="15" t="n">
         <v>39.4996</v>
@@ -1202,6 +1341,9 @@
       <c r="G45" s="16" t="n">
         <f aca="false">SUM(B45:F45)/5</f>
         <v>58.2586</v>
+      </c>
+      <c r="H45" s="13" t="n">
+        <v>49.915</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,61 +1354,114 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="16"/>
+      <c r="H46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
+        <v>22</v>
+      </c>
+      <c r="B47" s="15" t="n">
+        <v>574.501</v>
+      </c>
+      <c r="C47" s="15" t="n">
+        <v>971.089</v>
+      </c>
+      <c r="D47" s="15" t="n">
+        <v>1132.22</v>
+      </c>
+      <c r="E47" s="15" t="n">
+        <v>598.387</v>
+      </c>
+      <c r="F47" s="15" t="n">
+        <v>1080.21</v>
+      </c>
       <c r="G47" s="16" t="n">
         <f aca="false">SUM(B47:F47)/5</f>
-        <v>0</v>
+        <v>871.2814</v>
+      </c>
+      <c r="H47" s="13" t="n">
+        <v>903.739</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
+        <v>23</v>
+      </c>
+      <c r="B48" s="15" t="n">
+        <v>592.749</v>
+      </c>
+      <c r="C48" s="15" t="n">
+        <v>987.562</v>
+      </c>
+      <c r="D48" s="15" t="n">
+        <v>1154.12</v>
+      </c>
+      <c r="E48" s="15" t="n">
+        <v>612.06</v>
+      </c>
+      <c r="F48" s="15" t="n">
+        <v>1116.77</v>
+      </c>
       <c r="G48" s="16" t="n">
         <f aca="false">SUM(B48:F48)/5</f>
-        <v>0</v>
+        <v>892.6522</v>
+      </c>
+      <c r="H48" s="13" t="n">
+        <v>880.252</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
+        <v>24</v>
+      </c>
+      <c r="B49" s="15" t="n">
+        <v>360.202</v>
+      </c>
+      <c r="C49" s="15" t="n">
+        <v>640.322</v>
+      </c>
+      <c r="D49" s="15" t="n">
+        <v>639.195</v>
+      </c>
+      <c r="E49" s="15" t="n">
+        <v>354.701</v>
+      </c>
+      <c r="F49" s="15" t="n">
+        <v>674.669</v>
+      </c>
       <c r="G49" s="16" t="n">
         <f aca="false">SUM(B49:F49)/5</f>
-        <v>0</v>
+        <v>533.8178</v>
+      </c>
+      <c r="H49" s="13" t="n">
+        <v>546.499</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="B50" s="15" t="n">
+        <v>240.909</v>
+      </c>
+      <c r="C50" s="15" t="n">
+        <v>517.775</v>
+      </c>
+      <c r="D50" s="15" t="n">
+        <v>409.219</v>
+      </c>
+      <c r="E50" s="15" t="n">
+        <v>198.443</v>
+      </c>
+      <c r="F50" s="15" t="n">
+        <v>410.039</v>
+      </c>
       <c r="G50" s="16" t="n">
         <f aca="false">SUM(B50:F50)/5</f>
-        <v>0</v>
+        <v>355.277</v>
+      </c>
+      <c r="H50" s="13" t="n">
+        <v>372.532</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,10 +1472,11 @@
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
       <c r="G51" s="18"/>
+      <c r="H51" s="13"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B52" s="10" t="n">
         <v>10246893</v>
@@ -1298,6 +1494,7 @@
         <v>5450530</v>
       </c>
       <c r="G52" s="12"/>
+      <c r="H52" s="13"/>
     </row>
     <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>